<commit_message>
Generar excel matriz de caracterirticas
</commit_message>
<xml_diff>
--- a/url_data_clean.xlsx
+++ b/url_data_clean.xlsx
@@ -8,20 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JHON\Desktop\Nueva carpeta\scraping_data_seo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1237E35C-9D1E-42B2-ADB3-EB41F6BA753F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE16DC85-26D1-42D0-960F-A17AD8EA4A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="2355" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SEO_ALTO" sheetId="1" r:id="rId1"/>
     <sheet name="SEO_BAJO" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SEO_ALTO!$A$1:$A$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SEO_BAJO!$A$1:$A$180</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="204">
   <si>
     <t>SEO_ALTO</t>
   </si>
@@ -32,9 +36,6 @@
     <t>https://www.pclaptop.com.ec/</t>
   </si>
   <si>
-    <t>https://www.novicompu.com/computadoras</t>
-  </si>
-  <si>
     <t>https://store.nikotron.us/</t>
   </si>
   <si>
@@ -59,48 +60,21 @@
     <t>http://www.apctecnologia.com/</t>
   </si>
   <si>
-    <t>https://tenderati.com/ec/cc/electronica-y-tecnologia-en-guaranda/t/laptops</t>
-  </si>
-  <si>
-    <t>https://www.tiendeo.com.ec/guaranda/tecnologia-y-electronica</t>
-  </si>
-  <si>
-    <t>https://tenderati.com/ec/cc/electronica-y-tecnologia-en-tulcan/t/laptops</t>
-  </si>
-  <si>
-    <t>https://www.adfty.info/laptops/Ecuador/comprar-en-las-computadoras-portatiles-Tulcan.php</t>
-  </si>
-  <si>
-    <t>https://www.tiendeo.com.ec/tulcan/tecnologia-y-electr%C3%B3nica</t>
-  </si>
-  <si>
     <t>https://www.laptop.com.ec/</t>
   </si>
   <si>
     <t>https://systemarket.com.ec/</t>
   </si>
   <si>
-    <t>https://www.tiendeo.com.ec/riobamba/computron</t>
-  </si>
-  <si>
     <t>http://www.servicompu-rio.com/</t>
   </si>
   <si>
-    <t>https://tenderati.com/ec/cc/electronica-y-tecnologia-en-riobamba/t/portatiles-laptops</t>
-  </si>
-  <si>
-    <t>https://www.tiendeo.com.ec/latacunga/ofertas/laptop</t>
-  </si>
-  <si>
     <t>https://latacunga.doplim.ec/s/all-site/venta+laptop</t>
   </si>
   <si>
     <t>https://tecnomundoec.com/</t>
   </si>
   <si>
-    <t>https://tenderati.com/ec/cc/electronica-y-tecnologia-en-machala/t/portatiles-laptops</t>
-  </si>
-  <si>
     <t>https://www.aiyellow.com/accesorylaptops/</t>
   </si>
   <si>
@@ -116,15 +90,9 @@
     <t>https://www.iglobal.co/ecuador/galapagos/search-category/laptops-riobamba/2</t>
   </si>
   <si>
-    <t>https://www.hotelsolymar.com.ec/index.php/bloghotel/180-esta-pensado-en-visitar-las-maravillosas-islas-encantadas</t>
-  </si>
-  <si>
     <t>https://store.zigze.com/products/porta-laptop-tortuga-de-galapagos</t>
   </si>
   <si>
-    <t>https://www.kayak.com.ec/Puerto-Ayora-Hoteles-Ikala-Galapagos-Hotel.3731751.ksp</t>
-  </si>
-  <si>
     <t>https://www.worldcomputers.com.ec/</t>
   </si>
   <si>
@@ -134,12 +102,6 @@
     <t>https://www.creditoseconomicos.com/laptop</t>
   </si>
   <si>
-    <t>https://www.creditoseconomicos.com/tecnologia/computacion/laptops</t>
-  </si>
-  <si>
-    <t>https://www.tiendeo.com.ec/portoviejo/novicompu</t>
-  </si>
-  <si>
     <t>https://es.digitaltrends.com/computadoras/mejores-marcas-de-laptops/</t>
   </si>
   <si>
@@ -149,48 +111,21 @@
     <t>https://queportatilcomprar.net/mejores-marcas-portatiles/</t>
   </si>
   <si>
-    <t>https://www.magitech.pe/laptops/marcas.html</t>
-  </si>
-  <si>
     <t>https://pcacademia.com/las-mejores-marcas-de-laptops/</t>
   </si>
   <si>
     <t>https://laptop.com.pe/guia/las-7-mejores-marcas-de-laptop-2021/</t>
   </si>
   <si>
-    <t>https://www.iglobal.co/ecuador/tena/search-category/laptops-tena</t>
-  </si>
-  <si>
-    <t>https://indotrading.biz/laptops/Ecuador/portatil-Tena.php</t>
-  </si>
-  <si>
-    <t>https://www.tiendeo.com.ec/tena/ofertas/notebook</t>
-  </si>
-  <si>
     <t>https://www.ocompra.com/ecuador/item/laptop-asus-usada-431652518/</t>
   </si>
   <si>
     <t>https://vymaps.com/EC/Bull-Laptops-2251406931800835/</t>
   </si>
   <si>
-    <t>https://www.laptop.com.ec/local-centro-comercial-empresa-compra-venta-portatiles-computadores-pc-netbooks-notebooks-quito-ecuador.php</t>
-  </si>
-  <si>
-    <t>https://www.aiyellow.com/megacompucoca/</t>
-  </si>
-  <si>
     <t>https://www.importadoranovoa.com/</t>
   </si>
   <si>
-    <t>https://www.tiendeo.com.ec/puyo/ofertas/laptop</t>
-  </si>
-  <si>
-    <t>https://tenderati.com/ec/cc/electronica-y-tecnologia-en-puyo/t/laptop</t>
-  </si>
-  <si>
-    <t>https://www.iglobal.co/ecuador/puyo/search/ventas-de-laptop</t>
-  </si>
-  <si>
     <t>http://www.oascomputer.com/</t>
   </si>
   <si>
@@ -200,21 +135,12 @@
     <t>https://pcloja.com/producto/laptop-asus-x441uv-intel-core-i7-7500u/</t>
   </si>
   <si>
-    <t>https://www.marcimex.com/tecnologia/computadoras/laptops</t>
-  </si>
-  <si>
     <t>https://point.com.ec/</t>
   </si>
   <si>
-    <t>https://www.tiendeo.com.ec/loja/novicompu</t>
-  </si>
-  <si>
     <t>https://computron.com.ec/</t>
   </si>
   <si>
-    <t>https://point.com.ec/categoria-producto/tecnologia/laptops/</t>
-  </si>
-  <si>
     <t>https://techcomputer.ec/contacto/sucursal-ambato</t>
   </si>
   <si>
@@ -224,9 +150,6 @@
     <t>https://tenderati.com/ec/cc/electronica-y-tecnologia-en-ambato/t/portatiles-laptops</t>
   </si>
   <si>
-    <t>https://www.tiendeo.mx/zamora-de-hidalgo/ofertas/laptop</t>
-  </si>
-  <si>
     <t>https://www.marcimex.com/</t>
   </si>
   <si>
@@ -236,9 +159,6 @@
     <t>https://www.sams.com.mx/electronica-y-computacion/computo/laptops/_/N-8iu</t>
   </si>
   <si>
-    <t>https://catalogo.claro.com.ec/laptops-claro/web/index.php</t>
-  </si>
-  <si>
     <t>https://www.ubica.ec/explore/key/zamora/LAPTOP</t>
   </si>
   <si>
@@ -251,27 +171,15 @@
     <t>https://abclaptops.com/</t>
   </si>
   <si>
-    <t>https://tenderati.com/ec/cc/electronica-y-tecnologia-en-quito/t/portatiles-laptops</t>
-  </si>
-  <si>
-    <t>https://www.lenovo.com/ec/es/donde-comprar/distribuidores</t>
-  </si>
-  <si>
     <t>https://www.exacompu.com.ec/cambio-pantalla-laptop-quito/</t>
   </si>
   <si>
     <t>https://almacenesjapon.com/24-laptops</t>
   </si>
   <si>
-    <t>https://point.com.ec/categoria-producto/tecnologia/laptops/lenovo/</t>
-  </si>
-  <si>
     <t>https://compushop.ec/baterias-para-laptop/</t>
   </si>
   <si>
-    <t>https://tenderati.com/ec/cc/electronica-y-tecnologia-en-guayaquil/t/portatiles-laptops</t>
-  </si>
-  <si>
     <t>https://www.servicompu911.com/servicio-tecnico-laptops</t>
   </si>
   <si>
@@ -284,18 +192,9 @@
     <t>https://www.dell.com/es-ec</t>
   </si>
   <si>
-    <t>https://www.ganacell.com/computadoras</t>
-  </si>
-  <si>
     <t>https://gigacomputers.com.ec/</t>
   </si>
   <si>
-    <t>https://tenderati.com/ec/cc/electronica-y-tecnologia-en-cuenca/t/portatiles-laptops</t>
-  </si>
-  <si>
-    <t>https://www.tiendeo.com.ec/cuenca/ofertas/laptop</t>
-  </si>
-  <si>
     <t>https://www.compuplusec.com/</t>
   </si>
   <si>
@@ -317,9 +216,6 @@
     <t>https://www.iglobal.co/ecuador/guaranda/search-amp/laptops-quito</t>
   </si>
   <si>
-    <t>http://www.findglocal.com/EC/Unknown/1475263949444673/GABO-SYSTEMS-CORP</t>
-  </si>
-  <si>
     <t>https://www.computergloba.com/EC/Guaranda/66323</t>
   </si>
   <si>
@@ -335,9 +231,6 @@
     <t>http://www.orvehogar.com.ec/</t>
   </si>
   <si>
-    <t>https://www.jaher.com.ec/tiendas</t>
-  </si>
-  <si>
     <t>https://www.soyecuatoriano.com/guaranda-bolivar/audio+y+video</t>
   </si>
   <si>
@@ -347,30 +240,9 @@
     <t>https://www.globuya.com/EC/Guaranda/276870585715888/el-Capox-De-Las-Importaciones</t>
   </si>
   <si>
-    <t>https://www.tiendeo.com.ec/tulcan/ofertas/laptop</t>
-  </si>
-  <si>
-    <t>https://ec.placedigger.com/clinica-de-pcs-y-laptops54155509.html</t>
-  </si>
-  <si>
-    <t>https://www.yataco.com.pe/cargador-laptop/ciu.php?ciu=ec-tul&amp;key=Cargador-de-Laptop-Tulcan</t>
-  </si>
-  <si>
-    <t>http://todoesvirtual.com/index.php/2-gamers-ecuador-quito/19-precios-laptop-quito</t>
-  </si>
-  <si>
-    <t>https://www.tventas.com/</t>
-  </si>
-  <si>
-    <t>https://www.lanaciontv.ec/index.php/clasificados/item/5189-profesor-se-llevo-su-laptop-al-hospital-para-seguir-trabajando-y-muere-pocos-dias-despues</t>
-  </si>
-  <si>
     <t>https://www.ditronics.ec/</t>
   </si>
   <si>
-    <t>https://www.makemytrip.com/international-flights/tulcan-gulf_air-tickets.html</t>
-  </si>
-  <si>
     <t>https://eztradingcomputers.net/contact-us/</t>
   </si>
   <si>
@@ -380,15 +252,9 @@
     <t>https://www.nlarenas.com/2018/10/que-articulos-no-puedo-llevar-en-mi-equipaje-de-bodeja-o-en-cabina/</t>
   </si>
   <si>
-    <t>https://computron.com.ec/categories/impresoras_de_inyeccion/1816</t>
-  </si>
-  <si>
     <t>https://www.electrobahia.com.ec/categoria-producto/linea-tecnologica/computadoras/laptops/</t>
   </si>
   <si>
-    <t>https://www.iglobal.co/ecuador/search/laptops-riobamba</t>
-  </si>
-  <si>
     <t>https://dwsystems.business.site/</t>
   </si>
   <si>
@@ -398,33 +264,18 @@
     <t>https://ec.infoanuncios.com/computadoras-riobamba-portatiles-F1106C4071FD1</t>
   </si>
   <si>
-    <t>https://riobamba.doplim.ec/computadora-hp-a-10-venta-en-riobamba-id-941522.html</t>
-  </si>
-  <si>
     <t>https://www.findhealthclinics.com/EC/Riobamba/157890788044975/Libreria-y-Centro-De-Computo-Doctor-Pc</t>
   </si>
   <si>
     <t>https://cotopaxi.doplim.ec/s/all-site/laptops+en+latacunga</t>
   </si>
   <si>
-    <t>https://www.ubica.ec/info/CAPSCOMPU-VENTA-DE-COMPUTADORAS</t>
-  </si>
-  <si>
-    <t>https://www.iglobal.co/ecuador/latacunga/search-amp/laptops-quito</t>
-  </si>
-  <si>
-    <t>https://www.laptop.com.ec/novedades-nuevos-productos-compra-venta-portatiles-computadores-pc-netbooks-notebooks-quito-ecuador.php</t>
-  </si>
-  <si>
     <t>https://dealshaker.com/en/deal/sumycompu-laptop-asus-core-i5-1035g1-40-one-latacunga-ecuador/n5BPcp0v9fBV2V2vt8IpWUVpBVBHyiT6W2S10sOYEjU~</t>
   </si>
   <si>
     <t>https://ajpautotrader.com/search?c=14&amp;l=26084&amp;sc=16</t>
   </si>
   <si>
-    <t>https://www.tventas.com/content/12-catalogo-tventas</t>
-  </si>
-  <si>
     <t>https://www.costamarexpress.com/Servicios/Ecuador/Paquetes</t>
   </si>
   <si>
@@ -437,12 +288,6 @@
     <t>https://machalaonline.ec/categoria-producto/laptops/</t>
   </si>
   <si>
-    <t>https://www.tiendeo.com.ec/machala/computron</t>
-  </si>
-  <si>
-    <t>https://www.creditoseconomicos.com/tecnologia/computacion</t>
-  </si>
-  <si>
     <t>https://trionica.ec/</t>
   </si>
   <si>
@@ -452,9 +297,6 @@
     <t>https://www.bancomachala.com/</t>
   </si>
   <si>
-    <t>https://www.corcompu.com/index.php?id_category=17&amp;controller=category</t>
-  </si>
-  <si>
     <t>https://www.ganacell.com/laptop-evoo-2-en-12-pulg-touchscreen--blue--2gb--32gb--w10-773/p</t>
   </si>
   <si>
@@ -467,18 +309,9 @@
     <t>https://tienda.claro.com.ec/</t>
   </si>
   <si>
-    <t>https://www.coppel.com/coppel-granjas-esmeralda-371</t>
-  </si>
-  <si>
-    <t>https://www.hp.com/ec-es/home.html</t>
-  </si>
-  <si>
     <t>https://www.lacapital.com.mx/noticia/87646-Empate_a_ceros_dominical_en_el_Nemesio_Diez</t>
   </si>
   <si>
-    <t>https://www.lahora.com.ec/santo-domingo/mishell-roman-entrega-la-corona/</t>
-  </si>
-  <si>
     <t>https://www.jobtrainworks.org/east-palo-alto-career-center/</t>
   </si>
   <si>
@@ -488,9 +321,6 @@
     <t>https://www.galapagoslastminutes.com/es/cruise/camila-galapagos-trimaran/</t>
   </si>
   <si>
-    <t>https://galapagos.evisos.ec/s/laptop/sc-1</t>
-  </si>
-  <si>
     <t>http://www.galapagosaltamar.com/</t>
   </si>
   <si>
@@ -524,12 +354,6 @@
     <t>https://computron.com.ec/categories/laptops/41279</t>
   </si>
   <si>
-    <t>https://tenderati.com/ec/cc/electronica-y-tecnologia-en-ibarra/t/portatiles-laptops</t>
-  </si>
-  <si>
-    <t>https://www.aiyellow.com/laptopsylaptops/</t>
-  </si>
-  <si>
     <t>https://yellow.place/es/laptopsht-repuestos-ibarra-pantallas-cargadores-baterias-ibarra-ecuador</t>
   </si>
   <si>
@@ -542,9 +366,6 @@
     <t>https://es.cybo.com/EC-biz/hardtechnology-servicio-t%C3%A9cnico-de</t>
   </si>
   <si>
-    <t>https://www.tiendeo.com.ec/ibarra/ofertas/laptop</t>
-  </si>
-  <si>
     <t>https://www.guimun.com/ecuador/negociosec/4557/world-computers/contacto</t>
   </si>
   <si>
@@ -557,9 +378,6 @@
     <t>https://laptopssolutions.negocio.site/</t>
   </si>
   <si>
-    <t>https://www.tecnosmart.com.ec/categoria-producto/computadoras/laptops/</t>
-  </si>
-  <si>
     <t>http://www.elpaseoshopping.com/babahoyo/tecnologia/compu-tienda</t>
   </si>
   <si>
@@ -575,21 +393,12 @@
     <t>http://www.findglocal.com/EC/Babahoyo/118908742135979/Computer-House---Compmed-S.A</t>
   </si>
   <si>
-    <t>https://www.novicompu.com/celulares</t>
-  </si>
-  <si>
     <t>https://www.ganacell.com/</t>
   </si>
   <si>
-    <t>https://www.laptop.com.ec/novedades-nuevos-productos-compra-venta-portatiles-computadores-pc-netbooks-notebooks-quito-ecuador.php?tablajb=noticias&amp;p=19&amp;t=El-87por</t>
-  </si>
-  <si>
     <t>https://vymaps.com/EC/eGoTECH--laptop--Computadora--impresoras--345891/</t>
   </si>
   <si>
-    <t>https://www.travelocity.com/Cheap-Flights-To-Portoviejo.d2913.Travel-Guide-Flights</t>
-  </si>
-  <si>
     <t>https://www.expedia.co.kr/en/Cheap-Flights-To-Portoviejo.d2913.Travel-Guide-Flights</t>
   </si>
   <si>
@@ -632,9 +441,6 @@
     <t>https://www.doe.mass.edu/mcas/accessibility/guidelines.docx</t>
   </si>
   <si>
-    <t>https://www.redbubble.com/people/abzdraws/works/39864870-maca?p=laptop-sleeve</t>
-  </si>
-  <si>
     <t>https://www.laptopsdirect.co.uk/Mi_MACA_Colour_2200_Power_Case_for_iPhone_4-4S_-_Purple_SP103A-PL/version.asp</t>
   </si>
   <si>
@@ -644,9 +450,6 @@
     <t>https://www.promoplace.com/maca/computer-laptop-sleeves.htm</t>
   </si>
   <si>
-    <t>https://es.123rf.com/photo_75296462_jovem-mulher-bonita-com-um-laptop-e-uma-ma%C3%A7%C3%A3.html</t>
-  </si>
-  <si>
     <t>https://www.rit.edu/diversity/multicultural-center-academic-success-mcas</t>
   </si>
   <si>
@@ -680,18 +483,12 @@
     <t>https://www.walgreens.com/store/c/tena-men-incontinence,-protective-medium/large/ID=prod6327728-product</t>
   </si>
   <si>
-    <t>https://www.yataco.com.pe/teclado-laptop-hp/key-ciudad.php?o=4179&amp;c=ec-ten&amp;buscar=Teclado-HP-Stream-14-ax003ns-Tena-Teclado-para-laptop-HP</t>
-  </si>
-  <si>
     <t>https://www.redbubble.com/i/notebook/Tena-Slip-Diaper-by-Steve616/27273500.WX3NH</t>
   </si>
   <si>
     <t>https://teranews.net/mg/beelink-mii-v-replacement-for-pcs-and-laptops</t>
   </si>
   <si>
-    <t>https://www.novicompu.com/tiendas</t>
-  </si>
-  <si>
     <t>https://customers.microsoft.com/en-AU/story/grupo-sorolla-education-windows-autopilot-spain</t>
   </si>
   <si>
@@ -701,9 +498,6 @@
     <t>http://repositorio.ulvr.edu.ec/handle/44000/13</t>
   </si>
   <si>
-    <t>https://lv.yellowpages.net/phone,593-23819992,%C4%80rsts,Quito,ECEN134612.html</t>
-  </si>
-  <si>
     <t>https://co.hoteles.com/ho1091640160/apartamento-orellana-santa-margalida-espana/</t>
   </si>
   <si>
@@ -713,9 +507,6 @@
     <t>https://www.expedia.com/Cheap-Flights-To-Orellana-La-Vieja.d6357087.Travel-Guide-Flights</t>
   </si>
   <si>
-    <t>https://society6.com/product/sherlock-holmes-comic_laptop-skin</t>
-  </si>
-  <si>
     <t>https://unsplash.com/wallpapers/art</t>
   </si>
   <si>
@@ -725,27 +516,12 @@
     <t>https://www.cnet.com/tech/mobile/best-smartwatch/</t>
   </si>
   <si>
-    <t>https://www.bigrapidsnews.com/news/article/Honduras-presidential-candidate-arrested-16592997.php</t>
-  </si>
-  <si>
-    <t>https://centrosanmartino.com/is48v/rayb5uz.php?who=upcycle-bike-shop</t>
-  </si>
-  <si>
-    <t>https://tenderati.com/ec/cc/electronica-y-tecnologia-en-puyo/t/portatiles-laptops</t>
-  </si>
-  <si>
     <t>https://puyo.doplim.ec/s/servicios/reparacion+computadoras</t>
   </si>
   <si>
-    <t>https://www.nexdu.com/ec/puyo-y/empresa/pc-xpress-puyo-49992</t>
-  </si>
-  <si>
     <t>https://gringopost.com/2021/05/28/small-laptop-computer-in-the-us-needed-in-cuenca-or-puyo/</t>
   </si>
   <si>
-    <t>https://www.aiyellow.com/electrapctecnologia/</t>
-  </si>
-  <si>
     <t>https://www.pcgamebenchmark.com/puyo-puyo-tetris-system-requirements</t>
   </si>
   <si>
@@ -755,9 +531,6 @@
     <t>https://www.paginas-amarillas.com.ec/empresas/riofrio-lara-telecomunicaciones-cl/puyo-30866830</t>
   </si>
   <si>
-    <t>https://www.yataco.com.pe/servicio-tecnico-gamer/ciu.php?ciu=ec-puy&amp;key=Servicio-tecnico-de-Computadoras-Laptop-Gamer-Puyo</t>
-  </si>
-  <si>
     <t>https://bay-sell.com/search?l=13202&amp;c=14&amp;sc=16</t>
   </si>
   <si>
@@ -776,18 +549,9 @@
     <t>https://tienda.omega.com.do/es/category/list/141?type=grid</t>
   </si>
   <si>
-    <t>https://www.aiyellow.com/drlaptops/</t>
-  </si>
-  <si>
     <t>https://monsterlaptops.com.do/</t>
   </si>
   <si>
-    <t>https://www.xpc.com.do/servicios/ventas/equipos-tecnologico/ventas-computadoras.html</t>
-  </si>
-  <si>
-    <t>https://tenderati.com/ec/cc/electronica-y-tecnologia-en-santo-domingo/t/portatiles-laptops</t>
-  </si>
-  <si>
     <t>https://hooli.com.do/categoria-producto/computadoras/laptops/gaming-laptops/</t>
   </si>
   <si>
@@ -797,18 +561,9 @@
     <t>https://www.globatecrd.com/</t>
   </si>
   <si>
-    <t>https://www.tiendeo.com.ec/tiendas/santo-domingo/novicompu-av-quito-y-abraham-calazacon/95699</t>
-  </si>
-  <si>
     <t>https://doctorlaptoponline.com/</t>
   </si>
   <si>
-    <t>https://laptop.com.ec/empresa-compra-venta-portatiles-computadores-pc-netbooks-notebooks-quito-ecuador.php</t>
-  </si>
-  <si>
-    <t>https://repairloja.com/servicio-tecnico/hardware/laptops.html</t>
-  </si>
-  <si>
     <t>https://catalogo.claro.com.ec/laptops/catalogo</t>
   </si>
   <si>
@@ -827,27 +582,15 @@
     <t>https://www.lenovo.com/br/pt/laptops/c/LAPTOPS</t>
   </si>
   <si>
-    <t>https://www.dell.com/en-us/shop</t>
-  </si>
-  <si>
     <t>https://www.microsoft.com/en-us/store/b/pc</t>
   </si>
   <si>
-    <t>https://point.com.ec/producto/laptop-hp-14dk1002la-amd-athlon-3050u-8gb-ssd-256gb-14/</t>
-  </si>
-  <si>
-    <t>https://www.tiendeo.com.ec/ambato/novicompu</t>
-  </si>
-  <si>
     <t>https://puertolibreecuador.com/categoria-producto/computacion/laptops/</t>
   </si>
   <si>
     <t>https://virtualpcstore.com.ec/</t>
   </si>
   <si>
-    <t>https://horario.top/0644648/1800_-_Laptops</t>
-  </si>
-  <si>
     <t>https://www.nexdu.com/ec/ambato-t/empresa/1800-laptops-46198</t>
   </si>
   <si>
@@ -860,12 +603,6 @@
     <t>https://www.1800-laptops.com/</t>
   </si>
   <si>
-    <t>https://ambato.doplim.ec/reparacion-y-mantenimiento-de-computadores-y-laptops-id-443254.html</t>
-  </si>
-  <si>
-    <t>https://www.lenovo.com/ec/es/</t>
-  </si>
-  <si>
     <t>https://tiendas.guiabbb.ec/0124058/Compuservices_Ambato</t>
   </si>
   <si>
@@ -882,12 +619,6 @@
   </si>
   <si>
     <t>https://www.planetamexico.com.mx/zamora/venta+de+laptops</t>
-  </si>
-  <si>
-    <t>https://www.yataco.com.pe/cargador-laptop/ciu.php?ciu=ec-zam&amp;key=Cargador-de-Laptop-Zamora</t>
-  </si>
-  <si>
-    <t>https://www.mueblesamerica.mx/tecnologia/computadora/laptop.html</t>
   </si>
   <si>
     <t>https://lahora.com.ec/noticia/943558/roban-laptop-en-el-porvenir</t>
@@ -1269,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A73"/>
+  <dimension ref="A1:A45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A45" sqref="A8:A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,1685 +1015,1153 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A45" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A45">
+      <sortCondition ref="A1:A45"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A261"/>
+  <dimension ref="A1:A180"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>115</v>
+        <v>198</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>118</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>120</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>122</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>123</v>
+        <v>200</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>203</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>36</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>127</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>128</v>
+        <v>169</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>130</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>133</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>134</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>135</v>
+        <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>136</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>138</v>
+        <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>141</v>
+        <v>87</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>142</v>
+        <v>65</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>144</v>
+        <v>187</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>26</v>
+        <v>120</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>146</v>
+        <v>191</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>147</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>148</v>
+        <v>66</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>150</v>
+        <v>181</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>151</v>
+        <v>89</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>154</v>
+        <v>56</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>155</v>
+        <v>88</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>156</v>
+        <v>63</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>160</v>
+        <v>54</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>161</v>
+        <v>71</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>163</v>
+        <v>57</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>164</v>
+        <v>75</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>165</v>
+        <v>201</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>167</v>
+        <v>48</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>168</v>
+        <v>124</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>170</v>
+        <v>103</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>171</v>
+        <v>79</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>173</v>
+        <v>102</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>174</v>
+        <v>97</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>175</v>
+        <v>122</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>36</v>
+        <v>177</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>176</v>
+        <v>70</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>177</v>
+        <v>100</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>178</v>
+        <v>113</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>180</v>
+        <v>62</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>181</v>
+        <v>60</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>182</v>
+        <v>131</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>184</v>
+        <v>144</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>185</v>
+        <v>11</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>186</v>
+        <v>138</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>189</v>
+        <v>41</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>6</v>
+        <v>91</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>190</v>
+        <v>106</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>192</v>
+        <v>161</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>193</v>
+        <v>114</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>194</v>
+        <v>118</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>196</v>
+        <v>74</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>197</v>
+        <v>39</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>198</v>
+        <v>30</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>200</v>
+        <v>167</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>201</v>
+        <v>165</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>202</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>204</v>
+        <v>140</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>205</v>
+        <v>133</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>206</v>
+        <v>104</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>208</v>
+        <v>152</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>48</v>
+        <v>166</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>209</v>
+        <v>141</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>211</v>
+        <v>51</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>212</v>
+        <v>142</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>214</v>
+        <v>84</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>215</v>
+        <v>115</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>216</v>
+        <v>19</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>217</v>
+        <v>46</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>218</v>
+        <v>145</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>219</v>
+        <v>143</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>221</v>
+        <v>107</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>222</v>
+        <v>125</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>223</v>
+        <v>158</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>224</v>
+        <v>17</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>225</v>
+        <v>64</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>226</v>
+        <v>151</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>228</v>
+        <v>22</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>229</v>
+        <v>196</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A259" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" t="s">
-        <v>294</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A180" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A180">
+      <sortCondition ref="A1:A180"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>